<commit_message>
fix: fix a conflict
</commit_message>
<xml_diff>
--- a/serve/fast-api/file/test.xlsx
+++ b/serve/fast-api/file/test.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18288" windowHeight="9060"/>
+    <workbookView windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +29,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t>num</t>
+    <t>id</t>
   </si>
   <si>
     <t>name</t>
@@ -1225,7 +1225,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="4"/>

</xml_diff>